<commit_message>
Creation of Sequence Diagram from some use cases
</commit_message>
<xml_diff>
--- a/Fase_II/Use Cases/marcar como favorito.xlsx
+++ b/Fase_II/Use Cases/marcar como favorito.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nuno\Desktop\Li4---Sweetron\Fase_II\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nuno\Desktop\Li4---Sweetron\Fase_II\Use Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA09B506-1409-42EA-BAFD-D6812C9AA266}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62C1FAC-7243-4830-8233-5DA491976B55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="84" yWindow="456" windowWidth="25440" windowHeight="14724" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
@@ -61,10 +61,10 @@
     <t>Utilizador marca uma receita como favorita</t>
   </si>
   <si>
-    <t>1. Indica que quer marcar um produto como favorito</t>
-  </si>
-  <si>
     <t>2. Regista a receita como favorita</t>
+  </si>
+  <si>
+    <t>1. Indica que quer marcar uma receita como favorito</t>
   </si>
 </sst>
 </file>
@@ -260,6 +260,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -272,24 +288,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -611,7 +611,7 @@
   <dimension ref="B1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -627,65 +627,65 @@
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="5"/>
+      <c r="D3" s="11"/>
     </row>
     <row r="4" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="D4" s="11"/>
     </row>
     <row r="5" spans="2:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="7"/>
+      <c r="D5" s="13"/>
     </row>
     <row r="6" spans="2:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="36" x14ac:dyDescent="0.35">
-      <c r="B7" s="10"/>
-      <c r="C7" s="8" t="s">
-        <v>11</v>
+      <c r="B7" s="14"/>
+      <c r="C7" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="15"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="14" t="s">
-        <v>12</v>
+      <c r="D8" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C17" s="13"/>
+      <c r="C17" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>